<commit_message>
bug fixing add ticket from excel
</commit_message>
<xml_diff>
--- a/dist/ticketing/files/template_ticket_import.xlsx
+++ b/dist/ticketing/files/template_ticket_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F82113C-CF1C-4E74-9F8B-30C53C099DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC06697-242E-452A-B6FC-AB38649CB8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>hari_masuk</t>
   </si>
@@ -58,43 +58,34 @@
     <t>products_name</t>
   </si>
   <si>
-    <t>2024-06-01</t>
-  </si>
-  <si>
-    <t>2024-06-02</t>
-  </si>
-  <si>
     <t>08:00</t>
   </si>
   <si>
     <t>10:00</t>
   </si>
   <si>
-    <t>Kendala Sistem</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Tidak bisa login</t>
-  </si>
-  <si>
     <t>Reset password</t>
   </si>
   <si>
-    <t>08123456789</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
-    <t>Photobooth</t>
+    <t>Gugus Pangan</t>
+  </si>
+  <si>
+    <t>Selamat sore bapak saya briptu hariawan operator program 1 polrestabes surabaya mohon petunjuk apakah ada akun untuk admin polres untuk monitoring pelaporan bhabinkamtibmas polsek jajaran pada aplikasi gugus tugas polri ketahanan pangan  ?</t>
+  </si>
+  <si>
+    <t>melakukan koordinasi dengan tim internal aplikasi 13:59</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,9 +138,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -458,31 +460,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="78.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="32.42578125" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="4" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -506,7 +508,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -517,41 +519,35 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3">
+        <v>45466</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45467</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add places_id at import excel
</commit_message>
<xml_diff>
--- a/dist/ticketing/files/template_ticket_import.xlsx
+++ b/dist/ticketing/files/template_ticket_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC06697-242E-452A-B6FC-AB38649CB8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425CDAA1-95E2-4FA2-A72A-244020D5CF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>hari_masuk</t>
   </si>
@@ -58,9 +58,6 @@
     <t>products_name</t>
   </si>
   <si>
-    <t>08:00</t>
-  </si>
-  <si>
     <t>10:00</t>
   </si>
   <si>
@@ -77,6 +74,27 @@
   </si>
   <si>
     <t>melakukan koordinasi dengan tim internal aplikasi 13:59</t>
+  </si>
+  <si>
+    <t>081319107692</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Photobooth</t>
+  </si>
+  <si>
+    <t>places_id</t>
   </si>
 </sst>
 </file>
@@ -84,7 +102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -138,21 +156,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,97 +489,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="78.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="78.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="88.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>45466</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>45467</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="6">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45483</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45484</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="K3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
+      <c r="M3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>